<commit_message>
Changes to be committed: Forgot to add my own test file for my clue board. 	modified:   data/ClueLayout.xlsx 	modified:   data/ClueSetup.txt 	modified:   src/clueGame/BoardCell.java 	new file:   src/tests/FileInitTests.java
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\School\Fall 2020\CSCI306\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D2E437-2A58-4848-B7B5-37F3CD353443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBB3E59-699B-4371-B10B-4F390CAAD6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98A481F3-416E-411A-A8BB-D80C40E0FB0C}"/>
   </bookViews>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3AF44C-DFCC-4B44-9832-1BA6EA371032}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH23" sqref="AH23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,7 +996,7 @@
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1768,10 +1768,10 @@
       <c r="J18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="M18" s="3" t="s">

</xml_diff>

<commit_message>
Changes to be committed: Updated README for submission 	modified:   README.md Found error for one of the secret passage ways in CSV and XLSX 	modified:   data/ClueLayout.csv 	modified:   data/ClueLayout.xlsx Modified Board and BoardCell to pass tests 	modified:   src/clueGame/Board.java 	modified:   src/clueGame/BoardCell.java Some tests were incorrect and required correction 	modified:   src/tests/BoardAdjTargetTest.java
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\School\Fall 2020\CSCI306\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1000F63-A5C2-4085-868A-16DB45D638BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3F73AA-6EB6-447C-8913-3920AD25E1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98A481F3-416E-411A-A8BB-D80C40E0FB0C}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>L*</t>
   </si>
   <si>
-    <t>PL</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>Red: Test Occupied</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,7 +763,7 @@
         <v>21</v>
       </c>
       <c r="AB1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -820,16 +820,16 @@
         <v>2</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>0</v>
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
@@ -895,16 +895,16 @@
         <v>2</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="AB3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -970,16 +970,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T4" s="15" t="s">
-        <v>20</v>
-      </c>
       <c r="U4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>0</v>
@@ -1042,16 +1042,16 @@
         <v>2</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V5" s="2" t="s">
         <v>0</v>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -1069,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -1117,25 +1117,25 @@
         <v>2</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB6" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
@@ -1192,25 +1192,25 @@
         <v>2</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB7" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
@@ -1285,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="AB8" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
@@ -1294,22 +1294,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>2</v>
@@ -1366,22 +1366,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>2</v>
@@ -1414,22 +1414,22 @@
         <v>2</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
@@ -1438,22 +1438,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>2</v>
@@ -1486,22 +1486,22 @@
         <v>6</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
@@ -1510,22 +1510,22 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>2</v>
@@ -1558,22 +1558,22 @@
         <v>2</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
@@ -1582,10 +1582,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>3</v>
@@ -1630,22 +1630,22 @@
         <v>2</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="S13" s="6" t="s">
+      <c r="T13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="T13" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="U13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
@@ -1654,10 +1654,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>2</v>
@@ -1702,22 +1702,22 @@
         <v>2</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
@@ -1738,10 +1738,10 @@
         <v>2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>4</v>
@@ -1774,22 +1774,22 @@
         <v>2</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
@@ -1810,10 +1810,10 @@
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>2</v>
@@ -1846,22 +1846,22 @@
         <v>6</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
@@ -1870,10 +1870,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>2</v>
@@ -1882,10 +1882,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>2</v>
@@ -1918,22 +1918,22 @@
         <v>2</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
@@ -1942,10 +1942,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>2</v>
@@ -1954,10 +1954,10 @@
         <v>2</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>2</v>
@@ -2014,22 +2014,22 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>2</v>
@@ -2038,7 +2038,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>2</v>
@@ -2053,7 +2053,7 @@
         <v>2</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>2</v>
@@ -2086,46 +2086,46 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="K20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P20" s="3" t="s">
         <v>2</v>
@@ -2134,22 +2134,22 @@
         <v>6</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
@@ -2161,19 +2161,19 @@
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>2</v>
@@ -2182,46 +2182,46 @@
         <v>2</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="L21" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="M21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R21" s="1" t="s">
+      <c r="S21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S21" s="6" t="s">
+      <c r="T21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="T21" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="U21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
@@ -2242,10 +2242,10 @@
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>4</v>
@@ -2254,22 +2254,22 @@
         <v>6</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>4</v>
@@ -2278,22 +2278,22 @@
         <v>2</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
@@ -2326,22 +2326,22 @@
         <v>2</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>2</v>
@@ -2350,22 +2350,22 @@
         <v>2</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
@@ -2458,10 +2458,10 @@
         <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>4</v>
@@ -2521,19 +2521,19 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>2</v>
@@ -2542,22 +2542,22 @@
         <v>2</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L26" s="17" t="s">
         <v>2</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P26" s="3" t="s">
         <v>2</v>
@@ -2572,13 +2572,13 @@
         <v>2</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W26" s="17" t="s">
         <v>2</v>
@@ -2593,19 +2593,19 @@
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>2</v>
@@ -2614,22 +2614,22 @@
         <v>2</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P27" s="4" t="s">
         <v>4</v>
@@ -2638,22 +2638,22 @@
         <v>2</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
@@ -2662,22 +2662,22 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>2</v>
@@ -2686,22 +2686,22 @@
         <v>2</v>
       </c>
       <c r="J28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K28" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="L28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P28" s="3" t="s">
         <v>2</v>
@@ -2710,22 +2710,22 @@
         <v>2</v>
       </c>
       <c r="R28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S28" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S28" s="6" t="s">
+      <c r="T28" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="T28" s="18" t="s">
-        <v>16</v>
-      </c>
       <c r="U28" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
@@ -2734,22 +2734,22 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>2</v>
@@ -2758,22 +2758,22 @@
         <v>2</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P29" s="3" t="s">
         <v>2</v>
@@ -2782,22 +2782,22 @@
         <v>2</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
@@ -2806,22 +2806,22 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>2</v>
@@ -2830,22 +2830,22 @@
         <v>2</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P30" s="3" t="s">
         <v>2</v>
@@ -2854,10 +2854,10 @@
         <v>2</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T30" s="2" t="s">
         <v>0</v>
@@ -2866,10 +2866,10 @@
         <v>0</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -2878,22 +2878,22 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>2</v>
@@ -2902,22 +2902,22 @@
         <v>2</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P31" s="3" t="s">
         <v>2</v>
@@ -2926,10 +2926,10 @@
         <v>2</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T31" s="2" t="s">
         <v>0</v>
@@ -2938,10 +2938,10 @@
         <v>0</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
@@ -2950,22 +2950,22 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>2</v>
@@ -2974,22 +2974,22 @@
         <v>2</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P32" s="3" t="s">
         <v>2</v>
@@ -2998,10 +2998,10 @@
         <v>2</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T32" s="2" t="s">
         <v>0</v>
@@ -3022,19 +3022,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>3</v>
@@ -3046,22 +3046,22 @@
         <v>6</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P33" s="4" t="s">
         <v>4</v>
@@ -3070,10 +3070,10 @@
         <v>6</v>
       </c>
       <c r="R33" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T33" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Created the Control GUI class and implemented several functions to create it accord to a prefered layout. Also created setter functions to modify the data in the GUI
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\School\Fall 2020\CSCI306\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3F73AA-6EB6-447C-8913-3920AD25E1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B710A72A-A961-449E-AA2A-424312C328F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98A481F3-416E-411A-A8BB-D80C40E0FB0C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="52">
   <si>
     <t>X</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>PA</t>
+  </si>
+  <si>
+    <t>Blue: Starting Locations</t>
+  </si>
+  <si>
+    <t>W%</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +297,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -319,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -341,6 +353,8 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +677,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,8 +806,8 @@
       <c r="H2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>2</v>
+      <c r="I2" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>10</v>
@@ -813,8 +827,8 @@
       <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>2</v>
+      <c r="P2" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>2</v>
@@ -987,6 +1001,9 @@
       <c r="W4" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="AB4" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
@@ -1281,8 +1298,8 @@
       <c r="V8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="W8" s="3" t="s">
-        <v>2</v>
+      <c r="W8" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="AB8" s="20" t="s">
         <v>48</v>
@@ -1725,8 +1742,8 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
+      <c r="B15" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -2004,8 +2021,8 @@
       <c r="V18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="W18" s="3" t="s">
-        <v>2</v>
+      <c r="W18" s="22" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
@@ -2301,8 +2318,8 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>2</v>
+      <c r="B23" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Implemented Game Board GUI that scales and updates properly. Also cleaned up the known cards panel.
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\School\Fall 2020\CSCI306\ClueGame\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Java\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B710A72A-A961-449E-AA2A-424312C328F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF94353-907C-4B8F-89BA-F4908EBAE5F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98A481F3-416E-411A-A8BB-D80C40E0FB0C}"/>
+    <workbookView xWindow="-23148" yWindow="5532" windowWidth="23256" windowHeight="12576" xr2:uid="{98A481F3-416E-411A-A8BB-D80C40E0FB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="53">
   <si>
     <t>X</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>W%</t>
+  </si>
+  <si>
+    <t>W&lt;%</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +306,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -331,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -355,6 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,17 +687,17 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="3.5546875" customWidth="1"/>
-    <col min="9" max="9" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="3.5234375" customWidth="1"/>
+    <col min="9" max="9" width="3.5234375" customWidth="1"/>
     <col min="28" max="28" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="7">
         <f>COLUMN(A1)-1</f>
         <v>0</v>
@@ -780,7 +790,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7">
         <f>ROW(A1)-1</f>
         <v>0</v>
@@ -827,8 +837,8 @@
       <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="22" t="s">
-        <v>51</v>
+      <c r="P2" s="23" t="s">
+        <v>2</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>2</v>
@@ -855,7 +865,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7">
         <f t="shared" ref="A3:A33" si="1">ROW(A2)-1</f>
         <v>1</v>
@@ -863,8 +873,8 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -887,8 +897,8 @@
       <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>10</v>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>10</v>
@@ -930,7 +940,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -938,8 +948,8 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>9</v>
@@ -962,8 +972,8 @@
       <c r="J4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>11</v>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>12</v>
@@ -983,11 +993,11 @@
       <c r="Q4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="T4" s="15" t="s">
         <v>19</v>
@@ -1005,7 +1015,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1080,7 +1090,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1155,7 +1165,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1230,7 +1240,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1305,7 +1315,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1377,7 +1387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1449,7 +1459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1521,7 +1531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1593,7 +1603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1665,7 +1675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1737,7 +1747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1809,7 +1819,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1881,7 +1891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1953,7 +1963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2025,7 +2035,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -2097,7 +2107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -2169,7 +2179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -2241,7 +2251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -2313,7 +2323,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="7">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -2385,7 +2395,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="7">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -2457,7 +2467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="7">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -2529,7 +2539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="7">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -2601,7 +2611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="7">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -2673,7 +2683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="7">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -2681,8 +2691,8 @@
       <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>40</v>
+      <c r="C28" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>39</v>
@@ -2705,8 +2715,8 @@
       <c r="J28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="6" t="s">
-        <v>36</v>
+      <c r="K28" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>35</v>
@@ -2745,7 +2755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="7">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -2753,8 +2763,8 @@
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>39</v>
+      <c r="C29" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>41</v>
@@ -2777,8 +2787,8 @@
       <c r="J29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>35</v>
+      <c r="K29" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="L29" s="15" t="s">
         <v>37</v>
@@ -2817,7 +2827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="7">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -2889,7 +2899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="7">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -2961,7 +2971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="7">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -3033,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -3080,8 +3090,8 @@
       <c r="O33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P33" s="4" t="s">
-        <v>4</v>
+      <c r="P33" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="Q33" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added proper player movement
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Java\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF94353-907C-4B8F-89BA-F4908EBAE5F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BB2080-B0DB-46EC-8B2D-415B694E74B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5532" windowWidth="23256" windowHeight="12576" xr2:uid="{98A481F3-416E-411A-A8BB-D80C40E0FB0C}"/>
   </bookViews>
@@ -687,7 +687,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -795,7 +795,7 @@
         <f>ROW(A1)-1</f>
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -846,8 +846,8 @@
       <c r="R2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>17</v>
+      <c r="S2" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>17</v>
@@ -951,8 +951,8 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>9</v>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -975,8 +975,8 @@
       <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>12</v>
+      <c r="L4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>10</v>
@@ -999,8 +999,8 @@
       <c r="S4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="15" t="s">
-        <v>19</v>
+      <c r="T4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>17</v>
@@ -1026,8 +1026,8 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
+      <c r="D5" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
@@ -1125,8 +1125,8 @@
       <c r="K6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>10</v>
+      <c r="L6" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>10</v>
@@ -1398,8 +1398,8 @@
       <c r="C10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>22</v>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
@@ -1518,8 +1518,8 @@
       <c r="S11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>23</v>
+      <c r="T11" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>23</v>
@@ -1608,8 +1608,8 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
+      <c r="B13" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -1662,8 +1662,8 @@
       <c r="S13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="T13" s="6" t="s">
-        <v>25</v>
+      <c r="T13" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>23</v>
@@ -2214,8 +2214,8 @@
       <c r="K21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L21" s="13" t="s">
-        <v>31</v>
+      <c r="L21" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>29</v>
@@ -2238,8 +2238,8 @@
       <c r="S21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="T21" s="15" t="s">
-        <v>34</v>
+      <c r="T21" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>32</v>
@@ -2289,8 +2289,8 @@
       <c r="L22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>29</v>
+      <c r="M22" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>29</v>
@@ -2307,8 +2307,8 @@
       <c r="R22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>32</v>
+      <c r="S22" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>32</v>
@@ -2550,8 +2550,8 @@
       <c r="C26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>39</v>
+      <c r="D26" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>39</v>
@@ -2742,8 +2742,8 @@
       <c r="S28" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="T28" s="18" t="s">
-        <v>15</v>
+      <c r="T28" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="U28" s="1" t="s">
         <v>13</v>
@@ -2766,8 +2766,8 @@
       <c r="C29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>41</v>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>39</v>
@@ -2790,8 +2790,8 @@
       <c r="K29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L29" s="15" t="s">
-        <v>37</v>
+      <c r="L29" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>35</v>
@@ -2892,8 +2892,8 @@
       <c r="U30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="V30" s="1" t="s">
-        <v>13</v>
+      <c r="V30" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>13</v>
@@ -2937,8 +2937,8 @@
       <c r="L31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>35</v>
+      <c r="M31" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>35</v>

</xml_diff>